<commit_message>
v2 template with placeholdrs
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GlebV\Documents\tet\taurus-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FDA2E9-6958-42F8-BDB0-44EA086DEA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D252F6-B77E-4893-B3E1-A4390D91AC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="3540" windowWidth="23950" windowHeight="14630" xr2:uid="{5167B799-4833-4A16-96D1-4977E6B65D0C}"/>
+    <workbookView xWindow="8390" yWindow="3790" windowWidth="23950" windowHeight="14630" xr2:uid="{5167B799-4833-4A16-96D1-4977E6B65D0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Отчет" sheetId="1" r:id="rId1"/>
@@ -69,16 +69,16 @@
     <t>Подпись владельца</t>
   </si>
   <si>
-    <t>ГБУ «Ветуправление Тбилисского района» :</t>
-  </si>
-  <si>
-    <t>И.О. заведущего Марьинским ветучастком ГБУ «Ветуправление Тбилисского района»_______________     ___________       Сосна М.А.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Специалист __________________________________________________  Мезенцева Н.В.                      </t>
-  </si>
-  <si>
     <t>Подписи: представители государственного бюджетного учреждения ветеринарии подведомственного департаменту ветеринарии Краснодарского края</t>
+  </si>
+  <si>
+    <t>VET_DEP :</t>
+  </si>
+  <si>
+    <t>И.О. заведущего Марьинским ветучастком VET_DEP_______________     ___________       VET_CEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Специалист __________________________________________________  VET_DOC                     </t>
   </si>
 </sst>
 </file>
@@ -199,11 +199,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,7 +522,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -539,57 +539,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-    </row>
-    <row r="4" spans="1:10" ht="202" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="4" spans="1:10" ht="207" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="11" t="s">
         <v>10</v>
       </c>
     </row>
@@ -624,7 +624,7 @@
     </row>
     <row r="7" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -638,7 +638,7 @@
     </row>
     <row r="8" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -652,7 +652,7 @@
     </row>
     <row r="9" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -666,7 +666,7 @@
     </row>
     <row r="10" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>

</xml_diff>